<commit_message>
-Add scales and limits to description of tracks -Add possibility to reverse scales
</commit_message>
<xml_diff>
--- a/src/JupyterTollsPyScientist/tracks_description_base.xlsx
+++ b/src/JupyterTollsPyScientist/tracks_description_base.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764E66D3-7DAA-4337-95C2-BFD9A0E859A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04F95A3-9623-4B85-9F39-D31CD46964B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tracks_description" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
   <si>
     <t>main</t>
   </si>
@@ -246,6 +246,18 @@
   </si>
   <si>
     <t>DEPTH_MD, DEPT</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>reverse</t>
   </si>
 </sst>
 </file>
@@ -600,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A1:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,11 +625,10 @@
     <col min="3" max="3" width="19.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -645,8 +656,14 @@
       <c r="I1" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,10 +685,20 @@
       <c r="G2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>120</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,10 +720,20 @@
       <c r="G3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -718,10 +755,20 @@
       <c r="G4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -743,10 +790,20 @@
       <c r="G5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>25</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -768,10 +825,20 @@
       <c r="G6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H6" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -793,10 +860,20 @@
       <c r="G7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H7" s="1">
+        <v>40</v>
+      </c>
+      <c r="I7" s="1">
+        <v>140</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -818,10 +895,20 @@
       <c r="G8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H8" s="1">
+        <v>-0.15</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -843,10 +930,20 @@
       <c r="G9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>12</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -868,10 +965,20 @@
       <c r="G10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I10" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -893,10 +1000,20 @@
       <c r="G11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -918,10 +1035,20 @@
       <c r="G12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H12" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="I12" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -941,10 +1068,20 @@
         <v>33</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H13" s="1">
+        <v>-3</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -964,10 +1101,20 @@
         <v>34</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H14" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="I14" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K14" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -987,10 +1134,20 @@
         <v>35</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H15" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="I15" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K15" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1012,10 +1169,20 @@
       <c r="G16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1037,8 +1204,18 @@
       <c r="G17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="H17" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="I17" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1050,7 +1227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB96C568-0CC8-433B-ACDA-60F08BF53F33}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
-Add possibility auto define the scale of curve based on values 5% and 95% values.
</commit_message>
<xml_diff>
--- a/src/JupyterTollsPyScientist/tracks_description_base.xlsx
+++ b/src/JupyterTollsPyScientist/tracks_description_base.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04F95A3-9623-4B85-9F39-D31CD46964B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672C749E-4348-459B-80D4-29DE482D1E76}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="82">
   <si>
     <t>main</t>
   </si>
@@ -258,6 +258,15 @@
   </si>
   <si>
     <t>reverse</t>
+  </si>
+  <si>
+    <t>range_detection</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>manual</t>
   </si>
 </sst>
 </file>
@@ -612,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A1:K12"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,9 +635,10 @@
     <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -662,8 +672,11 @@
       <c r="K1" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,8 +710,11 @@
       <c r="K2" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,8 +748,11 @@
       <c r="K3" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -767,8 +786,11 @@
       <c r="K4" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -802,8 +824,11 @@
       <c r="K5" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -837,8 +862,11 @@
       <c r="K6" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -872,8 +900,11 @@
       <c r="K7" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -907,8 +938,11 @@
       <c r="K8" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -942,8 +976,11 @@
       <c r="K9" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -977,8 +1014,11 @@
       <c r="K10" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1012,8 +1052,11 @@
       <c r="K11" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1047,8 +1090,11 @@
       <c r="K12" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1080,8 +1126,11 @@
       <c r="K13" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1113,8 +1162,11 @@
       <c r="K14" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L14" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1146,8 +1198,11 @@
       <c r="K15" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1181,8 +1236,11 @@
       <c r="K16" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1215,6 +1273,9 @@
       </c>
       <c r="K17" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Adjust appropriate display of figure (bug in matplotlib related with dimensions changes).
</commit_message>
<xml_diff>
--- a/src/JupyterTollsPyScientist/tracks_description_base.xlsx
+++ b/src/JupyterTollsPyScientist/tracks_description_base.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EBB811-0349-4CB4-883C-0D466321E5F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F1903A-9963-443C-9FF2-C3292C5A4FEC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -863,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -939,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -1289,7 +1289,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>